<commit_message>
improved styling in check_form_functions and added a test to excel_test for strings
</commit_message>
<xml_diff>
--- a/tests/excel_tests/test.xlsx
+++ b/tests/excel_tests/test.xlsx
@@ -1,14 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2002A74-EA15-4812-9130-C681E5F6E55F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFC2F520-87D4-42B8-A064-F570BB888387}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="integer" sheetId="1" r:id="rId1"/>
+    <sheet name="strings" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -18,7 +19,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="14">
   <si>
     <t>A</t>
   </si>
@@ -41,6 +41,33 @@
   </si>
   <si>
     <t>fail</t>
+  </si>
+  <si>
+    <t>W/C</t>
+  </si>
+  <si>
+    <t>w/c</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> W/C</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> W/C </t>
+  </si>
+  <si>
+    <t xml:space="preserve">W / C </t>
+  </si>
+  <si>
+    <t>WC</t>
+  </si>
+  <si>
+    <t>W/C #0000000000</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>&lt;&lt;B4 is a space</t>
   </si>
 </sst>
 </file>
@@ -362,13 +389,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -376,7 +403,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -384,7 +411,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -392,12 +419,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -406,7 +433,7 @@
       </c>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -414,13 +441,98 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>3</v>
       </c>
       <c r="B7">
         <f>2*2</f>
         <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31BA5E2A-C5FC-4C26-AFC3-1950397B099B}">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="13.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ran new tests and fixed data_only flag in test_excel
</commit_message>
<xml_diff>
--- a/tests/excel_tests/test.xlsx
+++ b/tests/excel_tests/test.xlsx
@@ -3,13 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFC2F520-87D4-42B8-A064-F570BB888387}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D540534-752A-4DA3-9762-E6EAF5A98D70}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="integer" sheetId="1" r:id="rId1"/>
     <sheet name="strings" sheetId="2" r:id="rId2"/>
+    <sheet name="multi line cells" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="20">
   <si>
     <t>A</t>
   </si>
@@ -68,6 +69,30 @@
   </si>
   <si>
     <t>&lt;&lt;B4 is a space</t>
+  </si>
+  <si>
+    <t>line 1 line 2 line 3</t>
+  </si>
+  <si>
+    <t>line 1 
+line 2 
+line 3</t>
+  </si>
+  <si>
+    <t>line 1
+line 2
+line 3</t>
+  </si>
+  <si>
+    <t>wrap text</t>
+  </si>
+  <si>
+    <t>alt+enter
+w/spaces</t>
+  </si>
+  <si>
+    <t>alt+enter
+no spaces</t>
   </si>
 </sst>
 </file>
@@ -103,10 +128,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -459,7 +490,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31BA5E2A-C5FC-4C26-AFC3-1950397B099B}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -538,4 +569,64 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5178B3A5-C3BA-41E5-8DDE-BFD98DADC057}">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="11.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="3"/>
+    </row>
+    <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>